<commit_message>
latest 3-2-2022 read from Excel
</commit_message>
<xml_diff>
--- a/src/test/testdata/Book3.xlsx
+++ b/src/test/testdata/Book3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>1021132355&amp;</t>
+  </si>
+  <si>
+    <t>Amiraaa</t>
+  </si>
+  <si>
+    <t>1116332215&amp;</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -398,6 +404,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>